<commit_message>
ajout de scenarios à la fiche de test et mise à jour des designs
</commit_message>
<xml_diff>
--- a/Fiche de tests.xlsx
+++ b/Fiche de tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raf\Desktop\RobLip6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Scénario</t>
   </si>
@@ -113,16 +113,55 @@
     <t>Recherche de chemin</t>
   </si>
   <si>
-    <t>Interaction autonome avec l'environnement</t>
-  </si>
-  <si>
     <t>Saisir un objet donné</t>
   </si>
   <si>
     <t>Se déplacer vers un point sans heurter d'obstacle</t>
   </si>
   <si>
-    <t>Vérifier le comportement du robot en cas de changement de l'environnement: exemple: lancer une cannette</t>
+    <t>Interactions avec l'environnement</t>
+  </si>
+  <si>
+    <t>Numéro</t>
+  </si>
+  <si>
+    <t>Capteurs utilisés</t>
+  </si>
+  <si>
+    <t>élements externes utilisés</t>
+  </si>
+  <si>
+    <t>Caméra</t>
+  </si>
+  <si>
+    <t>éventuellement codes Aruco</t>
+  </si>
+  <si>
+    <t>QRCodes ou Aruco</t>
+  </si>
+  <si>
+    <t>Caméra + Lidar</t>
+  </si>
+  <si>
+    <t>Le robot doit saisir l'objet ayant un code</t>
+  </si>
+  <si>
+    <t>Le robot doit sortir d'une pièce tapisée de codes aruco tout seul</t>
+  </si>
+  <si>
+    <t>Tous les capteurs</t>
+  </si>
+  <si>
+    <t>Aucun</t>
+  </si>
+  <si>
+    <t>Le robot doit trouver le plus court chemin pour arriver à une destination décidée à l'avance</t>
+  </si>
+  <si>
+    <t>Aruco ou QRCode</t>
+  </si>
+  <si>
+    <t>Le robot doit suivre l'utilisateur qui porte un code</t>
   </si>
 </sst>
 </file>
@@ -138,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +193,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,21 +236,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -482,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,28 +569,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -533,25 +604,25 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -563,25 +634,25 @@
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -593,25 +664,25 @@
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -623,25 +694,25 @@
       <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -653,29 +724,101 @@
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="B14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>4</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>